<commit_message>
Nächste Schritte und Erledigte Meilensteine -Anna
</commit_message>
<xml_diff>
--- a/Statusbericht_BSP-v1.xlsx
+++ b/Statusbericht_BSP-v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\urauc\Documents\Ausbildung\FH\WFP\PM\wfp-pm-statusbericht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH_CS\Sem4\WFP\wfp-pm-statusbericht\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF3A617-7A62-43B2-9E1A-7E14907066A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4761DB35-55FE-4300-A196-861FB3768095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28905" yWindow="2820" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <r>
       <rPr>
@@ -255,6 +255,27 @@
     <t>* Krabbenfläche - flexible Breite oder fix? 
 * Punktesystem - Umrechnung von Krabbenbissen in Leben? Darstellung?
 * Okki Animiert: Optik, Position der Tentakel</t>
+  </si>
+  <si>
+    <t>Projektkoordination dokumentiert und abgeschlossen
+Projektcontrolling
+Networking auf der Party betrieben
+Projekt erfolgreich abgeschlossen</t>
+  </si>
+  <si>
+    <t>Design komplett und zur Einbindung in das Spiel übergeben
+Präsentables Spiel erzeugt
+Fortschritt durch Projektleiter als zumindest ausreichend bewertet
+Präsentation präsentierfertig vorbereitet
+Präsentation erfolgreich absolviert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grundidee gefunden 
+Projekt Pitch Kick Off
+Requirements festgelegt und priorisiert
+Techstack spezifizieren/ Technologien ausgewählt
+Spezifikation von Projektleiter approved
+Setup abgeschlossen </t>
   </si>
 </sst>
 </file>
@@ -912,24 +933,24 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.69921875" customWidth="1"/>
-    <col min="2" max="2" width="79.296875" customWidth="1"/>
-    <col min="3" max="3" width="16.19921875" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="79.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -938,40 +959,40 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="19"/>
     </row>
-    <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="19"/>
     </row>
-    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="19"/>
     </row>
-    <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="19"/>
     </row>
-    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="19"/>
     </row>
-    <row r="8" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -980,7 +1001,7 @@
       </c>
       <c r="C8" s="19"/>
     </row>
-    <row r="9" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="72.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
@@ -989,45 +1010,45 @@
       </c>
       <c r="C9" s="19"/>
     </row>
-    <row r="10" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="19"/>
     </row>
-    <row r="11" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="19"/>
     </row>
-    <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" ht="86.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="86.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" ht="169" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="168.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
@@ -1036,31 +1057,37 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
-      <c r="B19" s="13"/>
-    </row>
-    <row r="20" spans="1:3" ht="11.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
     </row>
-    <row r="21" spans="1:3" ht="73" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="16"/>
+      <c r="B21" s="16" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added my part :)
</commit_message>
<xml_diff>
--- a/Statusbericht_BSP-v1.xlsx
+++ b/Statusbericht_BSP-v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FH_CS\Sem4\WFP\wfp-pm-statusbericht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\source\repos\wfp-pm-statusbericht\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4761DB35-55FE-4300-A196-861FB3768095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7499F537-DF01-47FF-AE6C-D6D571C3784A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="2820" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <r>
       <rPr>
@@ -101,16 +101,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>von                              bis</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
@@ -122,58 +112,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="10"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">☐ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">kritisch
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">☐ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">teilweise kritisch
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">☐ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>planmäßig</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <b/>
         <sz val="10"/>
         <rFont val="Arial"/>
@@ -247,9 +185,6 @@
       </rPr>
       <t>Erledigte Meilensteine</t>
     </r>
-  </si>
-  <si>
-    <t>Joseph</t>
   </si>
   <si>
     <t>* Krabbenfläche - flexible Breite oder fix? 
@@ -277,12 +212,91 @@
 Spezifikation von Projektleiter approved
 Setup abgeschlossen </t>
   </si>
+  <si>
+    <t>OkkiGame</t>
+  </si>
+  <si>
+    <t>Anna Leitner, Ursula Rauch, Joseph Hangstein</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">☐ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">kritisch
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">☐ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>teilweise kritisch
+ x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>planmäßig</t>
+    </r>
+  </si>
+  <si>
+    <t>Leon Freudenthaler, Reinhard Rader</t>
+  </si>
+  <si>
+    <t>Ursula Rauch</t>
+  </si>
+  <si>
+    <t>von 15.4.2022 bis 16.05.2022</t>
+  </si>
+  <si>
+    <t>Recherche, Artwork Mockups, Umsetzung der Must-Requirements (Code)</t>
+  </si>
+  <si>
+    <t>Bisher durchweg positives Feedback von Projektbetreuer Freudenthaler. Probleme bei Implementierung der Artwork Mockups wurden besprochen und weitestgehend beseitigt. Meilensteinplan ist soweit adäquat. Krisen und eingetretene Risiken sind bisher keine aufgekommen.</t>
+  </si>
+  <si>
+    <t>Das Projekt verläuft bisher planmäßig. Die angestrebte Erledigung der Must Requirements ist so gut wie abgeschlossen: Ein rudimentäres Demolevel für das Spiel ist erstellt, die Bewegungslogik funktioniert, und handgezeichnete Modelle sind implementiert. Vorausgreifend wurde sogar schon Hit Recognition für den Player Character implementiert.</t>
+  </si>
+  <si>
+    <t>Aufgrund von Problemen bei der Implementation von Artwork Sprites in die Game Engine (Scaling war off) entstand eine zusätzliche Arbeit von insgesamt 8 Stunden, deren Gesamtkosten sich auf 240 Euro belaufen. Ebenso gestaltete sich die Umsetzung des Grappling Hooks als schwieriger als gedacht - statt den von Teammitglied Hangstein beanstandeten 5 Stunden Arbeitszeit benötigte dieser 15 Stunden. Dies bedeutet eine zusätzliche Kostenlast von 300 Euro. Die weiteren Ausgaben bewegen sich im vorhergesehenen Rahmen und entsprechen in etwa den vorausgesagten Kosten.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -296,10 +310,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
@@ -325,6 +335,23 @@
       <name val="Segoe UI Symbol"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -481,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -512,12 +539,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="11"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -541,6 +562,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="11"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -932,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -944,85 +977,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="19" t="s">
-        <v>17</v>
-      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="19"/>
+      <c r="B3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="19"/>
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="17"/>
     </row>
     <row r="5" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="19"/>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="17"/>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="19"/>
+      <c r="B6" s="18">
+        <v>44697</v>
+      </c>
+      <c r="C6" s="17"/>
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
-      <c r="C7" s="19"/>
+      <c r="C7" s="17"/>
     </row>
     <row r="8" spans="1:3" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="19"/>
+      <c r="B8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:3" ht="72.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="19"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" ht="29.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="19"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="17"/>
     </row>
     <row r="11" spans="1:3" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="19"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="17"/>
     </row>
     <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
@@ -1031,16 +1076,20 @@
     </row>
     <row r="13" spans="1:3" ht="86.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="168.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="13"/>
+        <v>11</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>28</v>
+      </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1050,10 +1099,10 @@
     </row>
     <row r="16" spans="1:3" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -1064,17 +1113,17 @@
     </row>
     <row r="18" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="13" t="s">
-        <v>19</v>
+      <c r="A19" s="12"/>
+      <c r="B19" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1082,11 +1131,11 @@
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>21</v>
+      <c r="A21" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1095,6 +1144,7 @@
     <mergeCell ref="C2:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>